<commit_message>
Split the dequeue service into 2 different services, added a new action: add study
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Project_link_samples_v4_0_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Project_link_samples_v4_0_0.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Project link samples Template</t>
   </si>
@@ -38,7 +38,7 @@
     <t>Study</t>
   </si>
   <si>
-    <t>Workflow Step Start</t>
+    <t>Workflow Step Order</t>
   </si>
   <si>
     <t>Sample Name</t>
@@ -50,7 +50,10 @@
     <t>Sample Container Coord</t>
   </si>
   <si>
-    <t>Add to project and/or study</t>
+    <t>Add to project</t>
+  </si>
+  <si>
+    <t>Add to study</t>
   </si>
   <si>
     <t>Remove from project</t>
@@ -91,7 +94,7 @@
     <font>
       <b val="1"/>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -102,7 +105,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -126,7 +129,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -159,35 +162,35 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -204,26 +207,26 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -240,67 +243,67 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -320,12 +323,12 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffbfbfbf"/>
       <rgbColor rgb="ff92d050"/>
       <rgbColor rgb="ffffd966"/>
       <rgbColor rgb="ff6fa8dc"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -524,12 +527,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -562,10 +565,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -813,12 +816,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1133,10 +1136,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1393,7 +1396,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="23.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1719" style="1" customWidth="1"/>
     <col min="2" max="5" width="22.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="1" customWidth="1"/>
     <col min="7" max="8" width="22.3516" style="1" customWidth="1"/>
@@ -4497,7 +4500,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A307">
-      <formula1>",Add to project and/or study,Remove from project,Remove from study"</formula1>
+      <formula1>",Add to project,Add to study,Remove from project,Remove from study"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4510,13 +4513,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="24.4141" style="21" customWidth="1"/>
+    <col min="1" max="1" width="24.5" style="21" customWidth="1"/>
     <col min="2" max="5" width="9.35156" style="21" customWidth="1"/>
     <col min="6" max="16384" width="12.6719" style="21" customWidth="1"/>
   </cols>
@@ -4558,7 +4561,9 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="19"/>
+      <c r="A5" t="s" s="18">
+        <v>15</v>
+      </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -4627,19 +4632,26 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
+    <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="19"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" ht="13.5" customHeight="1">
+    <row r="16" ht="15" customHeight="1">
       <c r="A16" s="19"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
+    </row>
+    <row r="17" ht="13.5" customHeight="1">
+      <c r="A17" s="19"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>